<commit_message>
Update on 20181114.2334 by YKBKyle
</commit_message>
<xml_diff>
--- a/RNote.xlsx
+++ b/RNote.xlsx
@@ -9,10 +9,10 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="1380" yWindow="4580" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="工作表1" sheetId="1" r:id="rId1"/>
+    <sheet name="RCommands" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,19 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
-  <si>
-    <t>commands</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>example</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>description</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -57,11 +45,131 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>class</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>package operation</t>
+    <t>Commands</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Example</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Description</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Learning Resources</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>http://www.statmethods.net/management/merging.html</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Data Management</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package Operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Other</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total &lt;- merge(data frame A, data frame B, by = "ID")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge 2 data frames by ID</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>total &lt;- merge(data frame A, data frame B, by =c("ID","Country"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>merge 2 data frames by ID and Country</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>packageVersion("Package")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>check the version of the loaded package</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package Operation</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_df()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>tbl_df(data frame A)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select(data frame A, ColVar1, ColVar2, ColVar3)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset only 3 columns of A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>convert date frame to tibble(data frame tbl)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select(data frame A, ColVar1:ColVarN)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> subset all columns starting from ColVar1 and ending with ColVarN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select(data frame A, -(ColVar1:ColVarN))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset all columns except those from ColVar1 to ColVarN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter(data frame A, ColVar &gt; 0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset all rows where ColVar &gt; 0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -69,7 +177,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -90,6 +198,15 @@
       <color theme="1"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="DengXian"/>
+      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -108,17 +225,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="超链接" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
@@ -393,56 +518,174 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.1640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="48" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.83203125" style="1"/>
+    <col min="2" max="2" width="68.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="E1" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
+      <c r="E3" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="2"/>
+      <c r="B6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="2"/>
+      <c r="B9" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="E9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="2"/>
+      <c r="B10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>33</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="A8:A10"/>
+    <mergeCell ref="E8:E10"/>
+  </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="D5" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update on 20181115.1408 by YKBKyle
</commit_message>
<xml_diff>
--- a/RNote.xlsx
+++ b/RNote.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="4580" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="RCommands" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -81,10 +81,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>Other</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>total &lt;- merge(data frame A, data frame B, by = "ID")</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -170,6 +166,246 @@
   </si>
   <si>
     <t>subset all rows where ColVar &gt; 0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>filter(data frame A, ColVar1 == "String1", ColVar2 == "String2")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>subset all rows with more than 1 logical expression</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrange()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrange(data frame A, ColVar)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort the rows of A so that ColVar is in ascending order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrange(data frame A, desc(ColVar))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>sort the rows of A so that ColVar is in descending order</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrange(data frame A, ColVar1, ColVar2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first arrange by ColVar1, then by ColVar2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>first arrange by ColVar1 (ascending), then by ColVar2 (descending)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>arrange(data frame A, ColVar1, desc(ColVar2))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mutate()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mutate(data frame A, ColVarM = ColVar1 / 2^20)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mutate(data frame A, ColVarM = ColVar1/2, ColVarO = ColVarM/2)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add a column, ColVarM, into A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>add 2 columns, ColVarM and ColVarO, into A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>summarize()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>by_ColVar1 &lt;- group_by(data frame A, ColVar1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group_by()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>group A by its column variable ColVar1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n_distinct()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>same as length(unique(x))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>unique()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve">remove duplicate elements/rows </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>pack_sum &lt;- summarize(by_ColVar1,
+count = n(),
+unique = n_distinct(ip_id),
+countries = n_distinct(country),
+avg_bytes = mean(size))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>all operations are done for each group
+"count": created with n(), is the number of rows of each group.
+"unique": created with n_distinct(ip_id), is the number of unique ip_id for each group.
+"countries": similar to "unique".
+"avg_bytes": created with mean(size), is the mean of size for each group.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>General</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantile()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>quantile(A, c(0.3, 0.5, 0.9))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>get 30%, 50%, 90% quantile of A</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>n()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>number of rows in the current group, only be used from within summarise(), mutate() and filter()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: dplyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>%&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>cran %&gt;% group_by(package) %&gt;% summarize(count = n())</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>put the result before %&gt;% as the first argument into the function after %&gt;%</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: readr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: tidyr</t>
+  </si>
+  <si>
+    <t>Package: tidyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gather()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>gather(students, sex, count, -grade)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>The data argument, students, gives the name of the original dataset. The key and value arguments -- sex and count, respectively -- give the column names for our tidy dataset. The final argument, -grade, says that we want to gather all columns EXCEPT the grade column</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate(res, sex_class, c("sex","class"))</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>separate 1 column sex_class into 2 columns, sex and class
+it assumes that the values are separated by something other than a letter or number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>spread()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>do the oposite of separate()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Package: tidyr</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parse_number()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>parse_number("class5")</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return only the number</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bind_rows()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>bind_rows(A, B)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>return [A; B]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -229,8 +465,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -239,6 +478,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -518,173 +763,455 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="68.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="70.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="1"/>
+    <col min="1" max="1" width="20.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="70.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="99.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="F3"/>
+    </row>
+    <row r="4" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="F4"/>
+    </row>
+    <row r="5" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E9" s="4"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="2"/>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="1" t="s">
+      <c r="C10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="D10" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E7" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A9" s="2"/>
-      <c r="B9" s="1" t="s">
+      <c r="D12" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C9" s="1" t="s">
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E9" s="2"/>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-      <c r="B10" s="1" t="s">
+      <c r="D13" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="1" t="s">
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="E10" s="2"/>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A11" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" s="1" t="s">
+      <c r="C14" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D14" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="C11" s="1" t="s">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="E11" s="1" t="s">
-        <v>33</v>
+      <c r="D15" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A22" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C23" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="D23" s="5" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="5"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="5"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A28" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A29" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="F30"/>
+    </row>
+    <row r="31" spans="1:6" ht="54" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C31" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A34" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A35" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="A8:A10"/>
-    <mergeCell ref="E8:E10"/>
+  <mergeCells count="19">
+    <mergeCell ref="D32:D33"/>
+    <mergeCell ref="C32:C33"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="A32:A33"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="C23:C27"/>
+    <mergeCell ref="D23:D27"/>
+    <mergeCell ref="A16:A19"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="A23:A27"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="B11:B13"/>
+    <mergeCell ref="A11:A13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1"/>
+    <hyperlink ref="E8" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Update on 20181115.2017by YKBKyle
</commit_message>
<xml_diff>
--- a/RNote.xlsx
+++ b/RNote.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="97">
   <si>
     <t>rm(list=ls())</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -406,6 +406,22 @@
   </si>
   <si>
     <t>return [A; B]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read.csv()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read.csv("csv file",as.is=TRUE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>read csv file, and prevent character from being converted to factor class</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>File Management</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -763,10 +779,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F35"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.2"/>
@@ -1185,6 +1201,20 @@
       </c>
       <c r="D35" s="1" t="s">
         <v>89</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A36" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>